<commit_message>
added transactions due feature
</commit_message>
<xml_diff>
--- a/Kaas.xlsx
+++ b/Kaas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/omkar/Desktop/Kaas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Kaas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F2CE9D-2967-0349-9AC2-2271C33E4E43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4E0042-5ECC-4D6F-A2F6-6DDA108B3FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="accounts" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="184">
   <si>
     <t>Office rent</t>
   </si>
@@ -1186,7 +1186,21 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="14">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1590,24 +1604,24 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection sqref="A1:I37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.625" customWidth="1"/>
+    <col min="5" max="5" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="66" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>130</v>
       </c>
@@ -1636,7 +1650,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -1665,7 +1679,7 @@
         <v>179000</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -1694,7 +1708,7 @@
         <v>179000</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -1723,7 +1737,7 @@
         <v>179000</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -1752,7 +1766,7 @@
         <v>179000</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -1781,7 +1795,7 @@
         <v>179000</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -1810,7 +1824,7 @@
         <v>179000</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -1839,7 +1853,7 @@
         <v>179000</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -1868,7 +1882,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -1897,7 +1911,7 @@
         <v>90000</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -1926,7 +1940,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -1955,7 +1969,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -1984,7 +1998,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -2013,7 +2027,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -2042,7 +2056,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -2071,7 +2085,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -2100,7 +2114,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -2129,7 +2143,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -2158,7 +2172,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -2187,7 +2201,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -2216,7 +2230,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -2245,7 +2259,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="23" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -2274,7 +2288,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="24" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -2303,7 +2317,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="25" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -2332,7 +2346,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="26" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>25</v>
       </c>
@@ -2361,7 +2375,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>26</v>
       </c>
@@ -2390,7 +2404,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="28" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>27</v>
       </c>
@@ -2419,7 +2433,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="29" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>28</v>
       </c>
@@ -2448,7 +2462,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="30" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>29</v>
       </c>
@@ -2477,7 +2491,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="31" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>30</v>
       </c>
@@ -2506,7 +2520,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="32" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -2535,7 +2549,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="33" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -2564,7 +2578,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="34" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>33</v>
       </c>
@@ -2593,7 +2607,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>34</v>
       </c>
@@ -2622,7 +2636,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>35</v>
       </c>
@@ -2651,7 +2665,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>36</v>
       </c>
@@ -2704,28 +2718,28 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:M58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.1640625" customWidth="1"/>
-    <col min="8" max="8" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.6640625" customWidth="1"/>
-    <col min="13" max="13" width="11.6640625" customWidth="1"/>
+    <col min="1" max="1" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.125" customWidth="1"/>
+    <col min="8" max="8" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.625" customWidth="1"/>
+    <col min="11" max="11" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.625" customWidth="1"/>
+    <col min="13" max="13" width="11.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" s="2" customFormat="1" ht="42" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>124</v>
       </c>
@@ -2766,7 +2780,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -2807,7 +2821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -2848,7 +2862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -2889,7 +2903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -2930,7 +2944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -2971,7 +2985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -3012,7 +3026,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -3053,7 +3067,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -3094,7 +3108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -3135,7 +3149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -3176,7 +3190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -3217,7 +3231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -3258,7 +3272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -3299,7 +3313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -3340,7 +3354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -3381,7 +3395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -3422,7 +3436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -3463,7 +3477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -3504,7 +3518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -3545,7 +3559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -3586,7 +3600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -3627,7 +3641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -3668,7 +3682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -3709,7 +3723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -3750,7 +3764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>25</v>
       </c>
@@ -3791,7 +3805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>26</v>
       </c>
@@ -3832,7 +3846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>27</v>
       </c>
@@ -3873,7 +3887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>28</v>
       </c>
@@ -3914,7 +3928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>29</v>
       </c>
@@ -3955,7 +3969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>30</v>
       </c>
@@ -3996,7 +4010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -4037,7 +4051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -4078,7 +4092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>33</v>
       </c>
@@ -4119,7 +4133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>34</v>
       </c>
@@ -4160,7 +4174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>35</v>
       </c>
@@ -4201,7 +4215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>36</v>
       </c>
@@ -4242,7 +4256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>37</v>
       </c>
@@ -4283,7 +4297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>38</v>
       </c>
@@ -4324,7 +4338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>39</v>
       </c>
@@ -4365,7 +4379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>40</v>
       </c>
@@ -4406,7 +4420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>41</v>
       </c>
@@ -4447,7 +4461,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>42</v>
       </c>
@@ -4488,7 +4502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>43</v>
       </c>
@@ -4529,7 +4543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>44</v>
       </c>
@@ -4570,7 +4584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>45</v>
       </c>
@@ -4611,7 +4625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>46</v>
       </c>
@@ -4652,7 +4666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>47</v>
       </c>
@@ -4693,7 +4707,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>48</v>
       </c>
@@ -4734,7 +4748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>49</v>
       </c>
@@ -4775,7 +4789,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>50</v>
       </c>
@@ -4816,7 +4830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>51</v>
       </c>
@@ -4857,7 +4871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>52</v>
       </c>
@@ -4898,7 +4912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>53</v>
       </c>
@@ -4939,7 +4953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>54</v>
       </c>
@@ -4980,7 +4994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>55</v>
       </c>
@@ -5021,7 +5035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>56</v>
       </c>
@@ -5062,7 +5076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>57</v>
       </c>
@@ -5117,19 +5131,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C58">
-    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="Sals">
+    <cfRule type="containsText" dxfId="13" priority="7" operator="containsText" text="Sals">
       <formula>NOT(ISERROR(SEARCH("Sals",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="Servs">
+    <cfRule type="containsText" dxfId="12" priority="8" operator="containsText" text="Servs">
       <formula>NOT(ISERROR(SEARCH("Servs",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="Subs">
+    <cfRule type="containsText" dxfId="11" priority="9" operator="containsText" text="Subs">
       <formula>NOT(ISERROR(SEARCH("Subs",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="Bills">
+    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="Bills">
       <formula>NOT(ISERROR(SEARCH("Bills",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="Sals">
+    <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="Sals">
       <formula>NOT(ISERROR(SEARCH("Sals",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5154,23 +5168,23 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E58">
-    <cfRule type="containsText" dxfId="5" priority="90" operator="containsText" text="monthly">
+    <cfRule type="containsText" dxfId="7" priority="90" operator="containsText" text="monthly">
       <formula>NOT(ISERROR(SEARCH("monthly",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:G58">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Home">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Home">
       <formula>NOT(ISERROR(SEARCH("Home",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Office">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Office">
       <formula>NOT(ISERROR(SEARCH("Office",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18:G18">
-    <cfRule type="containsText" dxfId="1" priority="43" operator="containsText" text="Home">
+    <cfRule type="containsText" dxfId="3" priority="43" operator="containsText" text="Home">
       <formula>NOT(ISERROR(SEARCH("Home",F18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="44" operator="containsText" text="Office">
+    <cfRule type="containsText" dxfId="2" priority="44" operator="containsText" text="Office">
       <formula>NOT(ISERROR(SEARCH("Office",F18)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5219,18 +5233,18 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection sqref="A1:G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.5" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" customWidth="1"/>
+    <col min="6" max="6" width="10.875" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>173</v>
       </c>
@@ -5253,7 +5267,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>45116.693449074075</v>
       </c>
@@ -5266,8 +5280,17 @@
       <c r="D2" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E2" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G2" s="7">
+        <v>2953</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>45117</v>
       </c>
@@ -5280,8 +5303,17 @@
       <c r="D3" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E3" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="G3" s="7">
+        <v>2953</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>45118</v>
       </c>
@@ -5294,8 +5326,17 @@
       <c r="D4" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E4" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G4" s="7">
+        <v>2953</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>45119</v>
       </c>
@@ -5308,8 +5349,17 @@
       <c r="D5" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E5" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G5" s="7">
+        <v>2953</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>45120</v>
       </c>
@@ -5322,8 +5372,17 @@
       <c r="D6" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E6" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G6" s="7">
+        <v>2953</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>45121</v>
       </c>
@@ -5336,8 +5395,17 @@
       <c r="D7" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E7" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G7" s="7">
+        <v>2953</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>45122</v>
       </c>
@@ -5350,8 +5418,17 @@
       <c r="D8" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E8" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G8" s="7">
+        <v>2953</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>45123</v>
       </c>
@@ -5364,8 +5441,17 @@
       <c r="D9" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E9" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="G9" s="7">
+        <v>2953</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>45124</v>
       </c>
@@ -5378,8 +5464,17 @@
       <c r="D10" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E10" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G10" s="7">
+        <v>2953</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>45125</v>
       </c>
@@ -5392,8 +5487,17 @@
       <c r="D11" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E11" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G11" s="7">
+        <v>2953</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>45126</v>
       </c>
@@ -5406,8 +5510,17 @@
       <c r="D12" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E12" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G12" s="7">
+        <v>2953</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>45127</v>
       </c>
@@ -5420,8 +5533,17 @@
       <c r="D13" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E13" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="G13" s="7">
+        <v>2953</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>45128</v>
       </c>
@@ -5434,8 +5556,17 @@
       <c r="D14" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E14" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G14" s="7">
+        <v>2953</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>45129</v>
       </c>
@@ -5448,8 +5579,17 @@
       <c r="D15" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E15" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="G15" s="7">
+        <v>2953</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>45130</v>
       </c>
@@ -5462,8 +5602,17 @@
       <c r="D16" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G16" s="7">
+        <v>2953</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>45131</v>
       </c>
@@ -5476,8 +5625,17 @@
       <c r="D17" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G17" s="7">
+        <v>2953</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>45132</v>
       </c>
@@ -5490,8 +5648,17 @@
       <c r="D18" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G18" s="7">
+        <v>2953</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>45133</v>
       </c>
@@ -5504,8 +5671,17 @@
       <c r="D19" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="G19" s="7">
+        <v>2953</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>45134</v>
       </c>
@@ -5518,8 +5694,17 @@
       <c r="D20" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G20" s="7">
+        <v>2953</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>45135</v>
       </c>
@@ -5532,8 +5717,17 @@
       <c r="D21" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="G21" s="7">
+        <v>2953</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>45136</v>
       </c>
@@ -5546,8 +5740,26 @@
       <c r="D22" t="s">
         <v>120</v>
       </c>
+      <c r="E22" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G22" s="7">
+        <v>2953</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="20" type="noConversion"/>
+  <conditionalFormatting sqref="E2:E22">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Home">
+      <formula>NOT(ISERROR(SEARCH("Home",E2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Office">
+      <formula>NOT(ISERROR(SEARCH("Office",E2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>